<commit_message>
Update metadata with new profile/deprecated columns
</commit_message>
<xml_diff>
--- a/Data/indicator_metadata.xlsx
+++ b/Data/indicator_metadata.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd HH:mm:ss UTC"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -355,14 +355,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N90"/>
+  <dimension ref="A1:P90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="20.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1">
@@ -408,30 +408,40 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>anuario_entrega</t>
+          <t>anuario</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>profile</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>automated</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>script_version</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>last_run</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>script_notes</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>indicator_notes</t>
         </is>
@@ -471,7 +481,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2_Nov</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -479,15 +489,20 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
         <is>
           <t>v2025-10-29</t>
         </is>
       </c>
-      <c r="L2" s="2">
+      <c r="N2" s="2">
         <v>45960</v>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>automated fao but not centralized</t>
         </is>
@@ -532,7 +547,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2_Nov</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -540,15 +555,20 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
         <is>
           <t>v2025-10-29</t>
         </is>
       </c>
-      <c r="L3" s="2">
+      <c r="N3" s="2">
         <v>45959</v>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>automated fao but not centralized</t>
         </is>
@@ -586,20 +606,20 @@
           <t>2016</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
         <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L4" s="2">
+      <c r="N4" s="2">
         <v>45999</v>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
         </is>
@@ -672,28 +692,28 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2_Nov</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
         <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L6" s="2">
+      <c r="N6" s="2">
         <v>45968</v>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>changed data source from fra to cci_lc</t>
         </is>
@@ -733,23 +753,23 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2_Nov</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
         <is>
           <t>v2025-10-29</t>
         </is>
       </c>
-      <c r="L7" s="2">
+      <c r="N7" s="2">
         <v>45964</v>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>automated fao but not centralized</t>
         </is>
@@ -789,7 +809,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>2_Nov</t>
+          <t>Y</t>
         </is>
       </c>
     </row>
@@ -827,7 +847,12 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>2_Nov</t>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Y</t>
         </is>
       </c>
     </row>
@@ -865,7 +890,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>2_Nov</t>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Y</t>
         </is>
       </c>
     </row>
@@ -936,7 +966,12 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>2_Nov</t>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Y</t>
         </is>
       </c>
     </row>
@@ -974,7 +1009,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>2_Nov</t>
+          <t>Y</t>
         </is>
       </c>
     </row>
@@ -1017,23 +1052,23 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>1_Sept</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
         <is>
           <t>v2025-12-08</t>
         </is>
       </c>
-      <c r="L14" s="2">
+      <c r="N14" s="2">
         <v>45999</v>
       </c>
-      <c r="M14" t="inlineStr">
+      <c r="O14" t="inlineStr">
         <is>
           <t>add helper function for clean footnote ids</t>
         </is>
@@ -1078,7 +1113,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>1_Sept</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1086,15 +1121,20 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
         <is>
           <t>v2025-12-08</t>
         </is>
       </c>
-      <c r="L15" s="2">
+      <c r="N15" s="2">
         <v>46000</v>
       </c>
-      <c r="M15" t="inlineStr">
+      <c r="O15" t="inlineStr">
         <is>
           <t>add helper function for clean footnote ids</t>
         </is>
@@ -1134,23 +1174,23 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1_Sept</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
         <is>
           <t>v2025-12-08</t>
         </is>
       </c>
-      <c r="L16" s="2">
+      <c r="N16" s="2">
         <v>45999</v>
       </c>
-      <c r="M16" t="inlineStr">
+      <c r="O16" t="inlineStr">
         <is>
           <t>add helper function for clean footnote ids</t>
         </is>
@@ -1190,23 +1230,23 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>1_Sept</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
         <is>
           <t>v2025-12-08</t>
         </is>
       </c>
-      <c r="L17" s="2">
+      <c r="N17" s="2">
         <v>45999</v>
       </c>
-      <c r="M17" t="inlineStr">
+      <c r="O17" t="inlineStr">
         <is>
           <t>add helper function for clean footnote ids</t>
         </is>
@@ -1282,6 +1322,11 @@
           <t>2020</t>
         </is>
       </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20">
@@ -1317,10 +1362,15 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>1_Sept</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -1358,6 +1408,11 @@
           <t>2020</t>
         </is>
       </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22">
@@ -1396,6 +1451,11 @@
           <t>2020</t>
         </is>
       </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23">
@@ -1436,10 +1496,10 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>1_Sept</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -1484,10 +1544,15 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>1_Sept</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -1530,6 +1595,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26">
@@ -1568,6 +1638,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27">
@@ -1601,6 +1676,11 @@
           <t>2020</t>
         </is>
       </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28">
@@ -1636,10 +1716,15 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>1_Sept</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -1684,10 +1769,15 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>1_Sept</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -1727,10 +1817,15 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>1_Sept</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -1768,6 +1863,11 @@
           <t>2015</t>
         </is>
       </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32">
@@ -1803,10 +1903,15 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>1_Sept</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -1851,10 +1956,15 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>1_Sept</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -1899,10 +2009,15 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>1_Sept</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -1947,10 +2062,15 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>1_Sept</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -1990,10 +2110,10 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>1_Sept</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -2071,7 +2191,12 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>1_Sept</t>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Y</t>
         </is>
       </c>
     </row>
@@ -2208,23 +2333,23 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>2_Nov</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr">
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
         <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L42" s="2">
+      <c r="N42" s="2">
         <v>45968</v>
       </c>
-      <c r="M42" t="inlineStr">
+      <c r="O42" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
         </is>
@@ -2269,7 +2394,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>2_Nov</t>
+          <t>Y</t>
         </is>
       </c>
     </row>
@@ -2350,7 +2475,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>2_Nov</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -2358,15 +2483,20 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="K45" t="inlineStr">
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
         <is>
           <t>v2025-10-29</t>
         </is>
       </c>
-      <c r="L45" s="2">
+      <c r="N45" s="2">
         <v>45960</v>
       </c>
-      <c r="M45" t="inlineStr">
+      <c r="O45" t="inlineStr">
         <is>
           <t>automated fao but not centralized</t>
         </is>
@@ -2404,20 +2534,20 @@
           <t>2021</t>
         </is>
       </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
         <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L46" s="2">
+      <c r="N46" s="2">
         <v>45999</v>
       </c>
-      <c r="M46" t="inlineStr">
+      <c r="O46" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
         </is>
@@ -2462,7 +2592,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>2_Nov</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
@@ -2470,15 +2600,20 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="K47" t="inlineStr">
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
         <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L47" s="2">
+      <c r="N47" s="2">
         <v>45982</v>
       </c>
-      <c r="M47" t="inlineStr">
+      <c r="O47" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
         </is>
@@ -2523,7 +2658,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>2_Nov</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -2531,15 +2666,20 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="K48" t="inlineStr">
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
         <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L48" s="2">
+      <c r="N48" s="2">
         <v>45982</v>
       </c>
-      <c r="M48" t="inlineStr">
+      <c r="O48" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
         </is>
@@ -2579,7 +2719,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>2_Nov</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -2587,15 +2727,20 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="K49" t="inlineStr">
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
         <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L49" s="2">
+      <c r="N49" s="2">
         <v>45968</v>
       </c>
-      <c r="M49" t="inlineStr">
+      <c r="O49" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
         </is>
@@ -2635,23 +2780,23 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>2_Nov</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
         <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L50" s="2">
+      <c r="N50" s="2">
         <v>45968</v>
       </c>
-      <c r="M50" t="inlineStr">
+      <c r="O50" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
         </is>
@@ -2696,7 +2841,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>2_Nov</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
@@ -2704,15 +2849,20 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="K51" t="inlineStr">
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
         <is>
           <t>v2025-10-29</t>
         </is>
       </c>
-      <c r="L51" s="2">
+      <c r="N51" s="2">
         <v>45960</v>
       </c>
-      <c r="M51" t="inlineStr">
+      <c r="O51" t="inlineStr">
         <is>
           <t>automated fao but not centralized</t>
         </is>
@@ -2750,20 +2900,20 @@
           <t>2021</t>
         </is>
       </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
         <is>
           <t>v2025-12-08</t>
         </is>
       </c>
-      <c r="L52" s="2">
+      <c r="N52" s="2">
         <v>45999</v>
       </c>
-      <c r="M52" t="inlineStr">
+      <c r="O52" t="inlineStr">
         <is>
           <t>add helper function for clean footnote ids</t>
         </is>
@@ -2806,6 +2956,11 @@
           <t>2020</t>
         </is>
       </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54">
@@ -2846,23 +3001,23 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>2_Nov</t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr">
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
         <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L54" s="2">
+      <c r="N54" s="2">
         <v>45985</v>
       </c>
-      <c r="M54" t="inlineStr">
+      <c r="O54" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
         </is>
@@ -2902,23 +3057,23 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>2_Nov</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
         <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L55" s="2">
+      <c r="N55" s="2">
         <v>45985</v>
       </c>
-      <c r="M55" t="inlineStr">
+      <c r="O55" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
         </is>
@@ -2994,6 +3149,11 @@
           <t>2016</t>
         </is>
       </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58">
@@ -3034,7 +3194,7 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>1_Sept</t>
+          <t>Y</t>
         </is>
       </c>
     </row>
@@ -3255,15 +3415,20 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="K64" t="inlineStr">
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
         <is>
           <t>v2025-12-08</t>
         </is>
       </c>
-      <c r="L64" s="2">
+      <c r="N64" s="2">
         <v>46001</v>
       </c>
-      <c r="M64" t="inlineStr">
+      <c r="O64" t="inlineStr">
         <is>
           <t>add helper function for clean footnote ids</t>
         </is>
@@ -3344,20 +3509,20 @@
           <t>2020</t>
         </is>
       </c>
-      <c r="J66" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="K66" t="inlineStr">
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
         <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L66" s="2">
+      <c r="N66" s="2">
         <v>45980</v>
       </c>
-      <c r="M66" t="inlineStr">
+      <c r="O66" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
         </is>
@@ -3395,20 +3560,20 @@
           <t>2021</t>
         </is>
       </c>
-      <c r="J67" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="K67" t="inlineStr">
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
         <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L67" s="2">
+      <c r="N67" s="2">
         <v>45980</v>
       </c>
-      <c r="M67" t="inlineStr">
+      <c r="O67" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
         </is>
@@ -3446,20 +3611,20 @@
           <t>2021</t>
         </is>
       </c>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="K68" t="inlineStr">
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr">
         <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L68" s="2">
+      <c r="N68" s="2">
         <v>45980</v>
       </c>
-      <c r="M68" t="inlineStr">
+      <c r="O68" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
         </is>
@@ -3499,23 +3664,23 @@
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>2_Nov</t>
-        </is>
-      </c>
-      <c r="J69" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="K69" t="inlineStr">
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr">
         <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L69" s="2">
+      <c r="N69" s="2">
         <v>45974</v>
       </c>
-      <c r="M69" t="inlineStr">
+      <c r="O69" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
         </is>
@@ -3560,7 +3725,7 @@
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>2_Nov</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J70" t="inlineStr">
@@ -3568,15 +3733,20 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="K70" t="inlineStr">
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr">
         <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L70" s="2">
+      <c r="N70" s="2">
         <v>45981</v>
       </c>
-      <c r="M70" t="inlineStr">
+      <c r="O70" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
         </is>
@@ -3614,6 +3784,24 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>v2025-12-08</t>
+        </is>
+      </c>
+      <c r="N71" s="2">
+        <v>46003</v>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>add helper function for clean footnote ids</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72">
@@ -3654,7 +3842,7 @@
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>2_Nov</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J72" t="inlineStr">
@@ -3664,15 +3852,30 @@
       </c>
       <c r="K72" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L72" s="2">
+      <c r="N72" s="2">
         <v>45978</v>
       </c>
-      <c r="M72" t="inlineStr">
+      <c r="O72" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
+        </is>
+      </c>
+      <c r="P72" t="inlineStr">
+        <is>
+          <t>deprecated composite indicator; moved to 3158, 5649, 5650</t>
         </is>
       </c>
     </row>
@@ -3748,7 +3951,12 @@
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>2_Nov</t>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>Y</t>
         </is>
       </c>
     </row>
@@ -3786,7 +3994,7 @@
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>1_Sept</t>
+          <t>Y</t>
         </is>
       </c>
     </row>
@@ -3893,20 +4101,20 @@
           <t>2024</t>
         </is>
       </c>
-      <c r="J78" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="K78" t="inlineStr">
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr">
         <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L78" s="2">
+      <c r="N78" s="2">
         <v>45968</v>
       </c>
-      <c r="M78" t="inlineStr">
+      <c r="O78" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
         </is>
@@ -3949,20 +4157,20 @@
           <t>2024</t>
         </is>
       </c>
-      <c r="J79" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="K79" t="inlineStr">
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M79" t="inlineStr">
         <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L79" s="2">
+      <c r="N79" s="2">
         <v>45968</v>
       </c>
-      <c r="M79" t="inlineStr">
+      <c r="O79" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
         </is>
@@ -4005,20 +4213,20 @@
           <t>2024</t>
         </is>
       </c>
-      <c r="J80" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="K80" t="inlineStr">
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M80" t="inlineStr">
         <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L80" s="2">
+      <c r="N80" s="2">
         <v>45968</v>
       </c>
-      <c r="M80" t="inlineStr">
+      <c r="O80" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
         </is>
@@ -4030,7 +4238,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t xml:space="preserve">Economic cost of disasters, by type of disaster_x000D__x000D__x000D__x000D__x000D__x000D_
+          <t xml:space="preserve">Economic cost of disasters, by type of disaster_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 </t>
         </is>
       </c>
@@ -4064,7 +4272,7 @@
       </c>
       <c r="I81" t="inlineStr">
         <is>
-          <t>2_Nov</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J81" t="inlineStr">
@@ -4072,15 +4280,20 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="K81" t="inlineStr">
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M81" t="inlineStr">
         <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L81" s="2">
+      <c r="N81" s="2">
         <v>45986</v>
       </c>
-      <c r="M81" t="inlineStr">
+      <c r="O81" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
         </is>
@@ -4092,7 +4305,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t xml:space="preserve">Occurrence of climate change-related and geophysical disasters_x000D__x000D__x000D__x000D__x000D__x000D_
+          <t xml:space="preserve">Occurrence of climate change-related and geophysical disasters_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 </t>
         </is>
       </c>
@@ -4126,7 +4339,7 @@
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>2_Nov</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="J82" t="inlineStr">
@@ -4136,15 +4349,30 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
           <t>v2025-11-06</t>
         </is>
       </c>
-      <c r="L82" s="2">
+      <c r="N82" s="2">
         <v>45973</v>
       </c>
-      <c r="M82" t="inlineStr">
+      <c r="O82" t="inlineStr">
         <is>
           <t>transition to centralized processing function</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>deprecated composite indicator; moved to 5645, 5646, 5647</t>
         </is>
       </c>
     </row>
@@ -4312,6 +4540,11 @@
           <t>2020</t>
         </is>
       </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88">
@@ -4423,7 +4656,12 @@
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>2_Nov</t>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>Y</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update metadata post olade reprocessing
</commit_message>
<xml_diff>
--- a/Data/indicator_metadata.xlsx
+++ b/Data/indicator_metadata.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd HH:mm:ss UTC"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -1375,6 +1375,19 @@
           <t>Y</t>
         </is>
       </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>v2025-12-29</t>
+        </is>
+      </c>
+      <c r="N20" s="2">
+        <v>46020</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>add remove_lac parameter to preserve source LAC data</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21">
@@ -1504,6 +1517,19 @@
           <t>Y</t>
         </is>
       </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>v2025-12-29</t>
+        </is>
+      </c>
+      <c r="N23" s="2">
+        <v>46021</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>add remove_lac parameter to preserve source LAC data</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24">
@@ -1557,6 +1583,19 @@
           <t>Y</t>
         </is>
       </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>v2025-12-29</t>
+        </is>
+      </c>
+      <c r="N24" s="2">
+        <v>46021</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>add remove_lac parameter to preserve source LAC data</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25">
@@ -1729,6 +1768,19 @@
           <t>Y</t>
         </is>
       </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>v2025-12-29</t>
+        </is>
+      </c>
+      <c r="N28" s="2">
+        <v>46021</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>add remove_lac parameter to preserve source LAC data</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29">
@@ -1782,6 +1834,19 @@
           <t>Y</t>
         </is>
       </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>v2025-12-29</t>
+        </is>
+      </c>
+      <c r="N29" s="2">
+        <v>46021</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>add remove_lac parameter to preserve source LAC data</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30">
@@ -1830,6 +1895,19 @@
           <t>Y</t>
         </is>
       </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>v2025-12-29</t>
+        </is>
+      </c>
+      <c r="N30" s="2">
+        <v>46020</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>add remove_lac parameter to preserve source LAC data</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31">
@@ -1916,6 +1994,19 @@
           <t>Y</t>
         </is>
       </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>v2025-12-29</t>
+        </is>
+      </c>
+      <c r="N32" s="2">
+        <v>46020</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>add remove_lac parameter to preserve source LAC data</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33">
@@ -1969,6 +2060,19 @@
           <t>Y</t>
         </is>
       </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>v2025-12-29</t>
+        </is>
+      </c>
+      <c r="N33" s="2">
+        <v>46021</v>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>add remove_lac parameter to preserve source LAC data</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34">
@@ -2022,6 +2126,19 @@
           <t>Y</t>
         </is>
       </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>v2025-12-29</t>
+        </is>
+      </c>
+      <c r="N34" s="2">
+        <v>46021</v>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>add remove_lac parameter to preserve source LAC data</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35">
@@ -2075,6 +2192,19 @@
           <t>Y</t>
         </is>
       </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>v2025-12-29</t>
+        </is>
+      </c>
+      <c r="N35" s="2">
+        <v>46021</v>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>add remove_lac parameter to preserve source LAC data</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36">
@@ -2118,6 +2248,19 @@
           <t>Y</t>
         </is>
       </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>v2025-12-29</t>
+        </is>
+      </c>
+      <c r="N36" s="2">
+        <v>46021</v>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>add remove_lac parameter to preserve source LAC data</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37">
@@ -3375,6 +3518,24 @@
       <c r="H63" t="inlineStr">
         <is>
           <t>2020</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>v2025-12-08</t>
+        </is>
+      </c>
+      <c r="N63" s="2">
+        <v>46020</v>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>add helper function for clean footnote ids</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update metadata after rerunning anuario olade indicators in dec 25
</commit_message>
<xml_diff>
--- a/Data/indicator_metadata.xlsx
+++ b/Data/indicator_metadata.xlsx
@@ -1381,7 +1381,7 @@
         </is>
       </c>
       <c r="N20" s="2">
-        <v>46020</v>
+        <v>46021</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1901,7 +1901,7 @@
         </is>
       </c>
       <c r="N30" s="2">
-        <v>46020</v>
+        <v>46021</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -2000,7 +2000,7 @@
         </is>
       </c>
       <c r="N32" s="2">
-        <v>46020</v>
+        <v>46021</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>

</xml_diff>